<commit_message>
renewing dataset and rmd files
</commit_message>
<xml_diff>
--- a/BulunTe_IphoneMonitor.xlsx
+++ b/BulunTe_IphoneMonitor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\U of Michigan\Winter 2024 Course\620\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\Documents\B-620-HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73CFC7D-A9BD-48DB-AE81-B2AFB8A33F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F5DAB9-A6FD-4053-8A73-73AC9216EDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5DCD145E-907B-4748-911F-90DF9DE12DC4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="83">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -300,6 +300,62 @@
   </si>
   <si>
     <t>2h19min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/27/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/28/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/29/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/30/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/31/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/1/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>59min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h12min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>53min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>38min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h10min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -673,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87610EBD-37D3-4AD0-89AC-A41D916B2B6C}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1124,7 +1180,7 @@
         <v>10</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:E28" si="2">IF(ISERROR(FIND("h", D18)), 0, LEFT(D18, FIND("h", D18)-1)*60) + IF(ISERROR(FIND("min", D18)), 0, MID(D18, IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1), FIND("min", D18) - IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1)))</f>
+        <f t="shared" ref="E18:E34" si="2">IF(ISERROR(FIND("h", D18)), 0, LEFT(D18, FIND("h", D18)-1)*60) + IF(ISERROR(FIND("min", D18)), 0, MID(D18, IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1), FIND("min", D18) - IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1)))</f>
         <v>63</v>
       </c>
       <c r="F18">
@@ -1192,7 +1248,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:C28" si="3">IF(ISERROR(FIND("h", B21)), 0, LEFT(B21, FIND("h", B21)-1)*60) + IF(ISERROR(FIND("min", B21)), 0, MID(B21, IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1), FIND("min", B21) - IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1)))</f>
+        <f t="shared" ref="C21:C34" si="3">IF(ISERROR(FIND("h", B21)), 0, LEFT(B21, FIND("h", B21)-1)*60) + IF(ISERROR(FIND("min", B21)), 0, MID(B21, IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1), FIND("min", B21) - IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1)))</f>
         <v>31</v>
       </c>
       <c r="D21" t="s">
@@ -1382,6 +1438,156 @@
       </c>
       <c r="G28" s="1">
         <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="F29">
+        <v>34</v>
+      </c>
+      <c r="G29" s="1">
+        <v>5.486111111111111E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>31</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>132</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F31">
+        <v>76</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.32222222222222224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="F32">
+        <v>85</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.32013888888888892</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="F33">
+        <v>57</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2.1527777777777781E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F34">
+        <v>84</v>
+      </c>
+      <c r="G34" s="1">
+        <v>9.7222222222222224E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>